<commit_message>
feat: Implementação do catalogo separado por categoria ou ordem alfabetica
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Castro\Documents\catalogo_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4241433D-2A95-455E-A995-E6CE62D75AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F068769D-A488-4501-A95F-1C762EF7937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02E3CDAF-A272-443C-8687-B38AE8A4CCA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
   <si>
     <t>ABRAC SELIM 31 8 ABSOLUTE AL PTO</t>
   </si>
@@ -33,27 +33,15 @@
     <t>ABRAC SELIM 31 8 IMP AL PTO</t>
   </si>
   <si>
-    <t>ABRA SELIM 31 8 IMP AL PTO</t>
-  </si>
-  <si>
-    <t>Nome do Produto</t>
-  </si>
-  <si>
     <t>Descrição</t>
   </si>
   <si>
-    <t>Preço</t>
-  </si>
-  <si>
     <t>78.0003</t>
   </si>
   <si>
     <t>78.0006</t>
   </si>
   <si>
-    <t>78.0005</t>
-  </si>
-  <si>
     <t>Código do Produto</t>
   </si>
   <si>
@@ -79,22 +67,227 @@
   </si>
   <si>
     <t xml:space="preserve">ADAPTADOR DE VALVULA ALUM 10PCS </t>
+  </si>
+  <si>
+    <t>79.0103</t>
+  </si>
+  <si>
+    <t>ADAPTADOR SUP GUIDAO PTO TAIWAN AHEAD 21 1</t>
+  </si>
+  <si>
+    <t>79.0220</t>
+  </si>
+  <si>
+    <t>ADAPTADOR SUP GUIDAO AL POL TAIWAN AHEAD 25 4</t>
+  </si>
+  <si>
+    <t>12.0050</t>
+  </si>
+  <si>
+    <t>ALAVANCA 12V SHIMANO DEORE M6100 S VISOR</t>
+  </si>
+  <si>
+    <t>12.0031</t>
+  </si>
+  <si>
+    <t>ALAVANCA 21V SHIMANO TX50</t>
+  </si>
+  <si>
+    <t>12.0030</t>
+  </si>
+  <si>
+    <t>ALAVANCA 2X9V SHIMANO ALTUS M2010</t>
+  </si>
+  <si>
+    <t>12.0047</t>
+  </si>
+  <si>
+    <t>ALAVANCA 3X7V ABSOLUTE K310</t>
+  </si>
+  <si>
+    <t>12.0019</t>
+  </si>
+  <si>
+    <t>ALAVANCA 3X7V SUNRACE M400</t>
+  </si>
+  <si>
+    <t>12.0048</t>
+  </si>
+  <si>
+    <t>ALAVANCA 3X8V ABSOLUTE K310</t>
+  </si>
+  <si>
+    <t>12.0041</t>
+  </si>
+  <si>
+    <t>ALAVANCA 3X8V SHIMANO ALTUS M315</t>
+  </si>
+  <si>
+    <t>12.0038</t>
+  </si>
+  <si>
+    <t>ALAVANCA 3X8 SUNRACE M503</t>
+  </si>
+  <si>
+    <t>12.0001</t>
+  </si>
+  <si>
+    <t>ALAVANCA AL YAMADA</t>
+  </si>
+  <si>
+    <t>12.0042</t>
+  </si>
+  <si>
+    <t>ALAVANCA DUPLA SUNRACE C10</t>
+  </si>
+  <si>
+    <t>12.0013</t>
+  </si>
+  <si>
+    <t>ALAVANCA EZ FIRE 21V SHIMANO EF 500 PTO</t>
+  </si>
+  <si>
+    <t>02.0033</t>
+  </si>
+  <si>
+    <t>RODA 16 AL RIMAXX NATURAL ESF PAR</t>
+  </si>
+  <si>
+    <t>02.0288</t>
+  </si>
+  <si>
+    <t>RODA 24 AERO VZAN PTO ESF PAR</t>
+  </si>
+  <si>
+    <t>02.0003</t>
+  </si>
+  <si>
+    <t>RODA 26 AERO VZAN PTO CUBO ROLLER PTO R FINO PAR</t>
+  </si>
+  <si>
+    <t>07.0051</t>
+  </si>
+  <si>
+    <t>PASTILHA REFIL ABSOLUTE ABS02S F DISCO REDONDA</t>
+  </si>
+  <si>
+    <t>44.0109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAMPA ESTRELA AH SET ABSOLUTE 5UN </t>
+  </si>
+  <si>
+    <t>12.0005</t>
+  </si>
+  <si>
+    <t>ALAVANCA EZ FIRE 21V AL YAMADA PTO</t>
+  </si>
+  <si>
+    <t>12.0046</t>
+  </si>
+  <si>
+    <t>ALAVANCA EZ FIRE 24V SUNRACE M406 PTO POL</t>
+  </si>
+  <si>
+    <t>12.0006</t>
+  </si>
+  <si>
+    <t>ALAVANCA EZ FIRE 24V YAMADA PTO</t>
+  </si>
+  <si>
+    <t>12.0011</t>
+  </si>
+  <si>
+    <t>ALAVANCA G SHIFT 21V YAMADA K30 INDEX</t>
+  </si>
+  <si>
+    <t>12.0002</t>
+  </si>
+  <si>
+    <t>ALAVANCA NYLON YAMADA</t>
+  </si>
+  <si>
+    <t>79.0194</t>
+  </si>
+  <si>
+    <t>AMORTECEDOR P QUADRO F SUSP 150MM PTA</t>
+  </si>
+  <si>
+    <t>79.0018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANEL ESPACADOR AL 10MM LISO PTO 10 PCS </t>
+  </si>
+  <si>
+    <t>44.0057</t>
+  </si>
+  <si>
+    <t>ARANHA ESTRELA P TAMPA AH SET 25 4</t>
+  </si>
+  <si>
+    <t>02.0260</t>
+  </si>
+  <si>
+    <t>ARO 16X1 75 RIMAXX AL NAT</t>
+  </si>
+  <si>
+    <t>02.0029</t>
+  </si>
+  <si>
+    <t>ARO 20 VZAN VMAXX 36F PTO VB S ILHOS</t>
+  </si>
+  <si>
+    <t>02.0030</t>
+  </si>
+  <si>
+    <t>ARO 20 VZAN VMAXX 36F BCO VB S ILHOS</t>
+  </si>
+  <si>
+    <t>02.0261</t>
+  </si>
+  <si>
+    <t>ARO 20X1 75 RIMAXX AL NAT</t>
+  </si>
+  <si>
+    <t>02.0058</t>
+  </si>
+  <si>
+    <t>ARO 20X1 75 VZAN AERO AZ</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>SELIM</t>
+  </si>
+  <si>
+    <t>ACESSÓRIOS</t>
+  </si>
+  <si>
+    <t>RODA</t>
+  </si>
+  <si>
+    <t>GUIDÃO</t>
+  </si>
+  <si>
+    <t>ALAVANCA</t>
+  </si>
+  <si>
+    <t>FREIO</t>
+  </si>
+  <si>
+    <t>QUADRO</t>
+  </si>
+  <si>
+    <t>MOVIMENTO DIREÇÃO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,11 +315,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,129 +634,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B5E345-C4B2-49FA-A914-04EE787905E0}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C2" sqref="C2:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>18</v>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>